<commit_message>
prep for tdd session
</commit_message>
<xml_diff>
--- a/Magic Squares.xlsx
+++ b/Magic Squares.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\magicbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B398904A-4AC8-4D1D-A6EB-353ABCF82E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138A2626-332D-4A0B-BC1B-138ABC924656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>rule 1 start with top center</t>
   </si>
@@ -121,12 +121,47 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>GENERAL RULE: You always try to go diagonally up towards the right</t>
+  </si>
+  <si>
+    <t>rule 4 if you out of the box from the right by following rule 2 you select the first column from the row above (immediate row)</t>
+  </si>
+  <si>
+    <t>rule 3 if you go out of the box from the top by following rule 2 you select the last row from that column (immediate column)</t>
+  </si>
+  <si>
+    <r>
+      <t>n(n^</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1)/2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -159,6 +194,34 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -297,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -353,11 +416,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,17 +642,19 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="59.6640625" customWidth="1"/>
+    <col min="5" max="5" width="69" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
+      <c r="B1" s="29" t="s">
+        <v>31</v>
+      </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -600,11 +665,11 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -613,12 +678,12 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -626,12 +691,12 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="B4" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="2" t="s">
@@ -643,12 +708,12 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="B5" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="2" t="s">
@@ -660,12 +725,12 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="2" t="s">
@@ -675,12 +740,12 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="2" t="s">
@@ -738,7 +803,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="26">
-        <f t="shared" ref="E11:E13" si="0">SUM(B11:D11)</f>
+        <f>SUM(B11:D11)</f>
         <v>15</v>
       </c>
       <c r="F11" s="1"/>
@@ -760,7 +825,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E12:E13" si="0">SUM(B12:D12)</f>
         <v>15</v>
       </c>
     </row>
@@ -818,7 +883,9 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="33" t="s">
+        <v>34</v>
+      </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -881,6 +948,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -889,10 +957,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -930,11 +998,11 @@
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -942,62 +1010,62 @@
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
@@ -1208,6 +1276,11 @@
       <c r="H19" s="9">
         <f>SUM(C14,D15,E16,F17,G18)</f>
         <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1260,11 +1333,11 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1273,67 +1346,67 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1633,11 +1706,11 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1648,75 +1721,75 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -2029,7 +2102,7 @@
       <c r="K19" s="2">
         <v>369</v>
       </c>
-      <c r="M19" s="31" t="s">
+      <c r="M19" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2763,12 +2836,12 @@
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2785,19 +2858,19 @@
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -2807,21 +2880,21 @@
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
         <v>9</v>
@@ -2829,21 +2902,21 @@
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
         <v>10</v>
@@ -2851,38 +2924,38 @@
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -2891,22 +2964,22 @@
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2931,19 +3004,19 @@
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -3480,20 +3553,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G3" s="1"/>

</xml_diff>